<commit_message>
fixed destructor to virtual, coding MyTalk proj
</commit_message>
<xml_diff>
--- a/projects/MyTalk/MyTalk_protol.xlsx
+++ b/projects/MyTalk/MyTalk_protol.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19620" windowHeight="8670"/>
+    <workbookView windowWidth="27840" windowHeight="13350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34">
   <si>
     <t xml:space="preserve">
 </t>
@@ -38,6 +38,12 @@
     <t>password</t>
   </si>
   <si>
+    <t>mark</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
     <t>friend</t>
   </si>
   <si>
@@ -59,15 +65,30 @@
     <t>nByte</t>
   </si>
   <si>
+    <t>login:</t>
+  </si>
+  <si>
+    <t>head(2byte)</t>
+  </si>
+  <si>
+    <t>0x0001</t>
+  </si>
+  <si>
     <t>注册流程：</t>
   </si>
   <si>
+    <t>account(srting)</t>
+  </si>
+  <si>
     <t>客户端发送注册消息</t>
   </si>
   <si>
     <t>消息分类：</t>
   </si>
   <si>
+    <t>password(string)</t>
+  </si>
+  <si>
     <t>服务端搜索有无用户，无用户就注册</t>
   </si>
   <si>
@@ -84,6 +105,18 @@
   </si>
   <si>
     <t>返回注册信息</t>
+  </si>
+  <si>
+    <t>login ack:</t>
+  </si>
+  <si>
+    <t>0x0002</t>
+  </si>
+  <si>
+    <t>isok(1byte)</t>
+  </si>
+  <si>
+    <t>0 is flase, 1 is ok</t>
   </si>
 </sst>
 </file>
@@ -92,8 +125,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -120,13 +153,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -143,6 +169,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -151,8 +191,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -166,69 +207,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,7 +225,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -252,6 +233,58 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -266,6 +299,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -278,25 +341,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,7 +419,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -320,133 +473,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,6 +511,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -487,17 +535,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -533,27 +577,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -562,145 +595,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1032,10 +1065,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:XFD16"/>
+  <dimension ref="A1:XFD18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1075,68 +1108,112 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
       </c>
       <c r="N5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="O5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="14:15">
       <c r="N6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="O6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="14:15">
       <c r="N7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="O7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="11" spans="14:14">
+      <c r="N11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="15:17">
+      <c r="O12" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="O13" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:15">
       <c r="B14" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H14" t="s">
-        <v>16</v>
+        <v>22</v>
+      </c>
+      <c r="O14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="2:13">
       <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14">
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="N16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="15:17">
+      <c r="O17" t="s">
         <v>17</v>
       </c>
-      <c r="I15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" t="s">
-        <v>20</v>
-      </c>
-      <c r="M15" t="s">
-        <v>21</v>
+      <c r="Q17" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="16" spans="2:2">
-      <c r="B16" t="s">
-        <v>22</v>
+    <row r="18" spans="15:17">
+      <c r="O18" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
coding MyTalk proj, fixed MyAddrInfo m_buf bug
</commit_message>
<xml_diff>
--- a/projects/MyTalk/MyTalk_protol.xlsx
+++ b/projects/MyTalk/MyTalk_protol.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25440" windowHeight="12225"/>
+    <workbookView windowWidth="25440" windowHeight="18735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
   <si>
     <t xml:space="preserve">
 </t>
@@ -153,6 +153,21 @@
   </si>
   <si>
     <t>0x02 ok, 0x03 repeat</t>
+  </si>
+  <si>
+    <t>send msg:</t>
+  </si>
+  <si>
+    <t>0x0004</t>
+  </si>
+  <si>
+    <t>src account(string)</t>
+  </si>
+  <si>
+    <t>dst account(string)</t>
+  </si>
+  <si>
+    <t>msg(string)</t>
   </si>
 </sst>
 </file>
@@ -160,12 +175,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -182,6 +197,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -189,6 +211,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -205,39 +234,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -249,6 +256,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -257,6 +272,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
@@ -264,6 +310,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -271,9 +325,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -294,37 +347,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -335,43 +357,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -383,133 +531,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,32 +560,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -603,6 +604,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -618,11 +634,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -631,152 +653,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -785,6 +807,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1101,10 +1126,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:XFD33"/>
+  <dimension ref="A1:XFD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1323,6 +1348,35 @@
       </c>
       <c r="Q33" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="14:14">
+      <c r="N37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="15:17">
+      <c r="O38" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="15:15">
+      <c r="O39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="15:15">
+      <c r="O40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="15:15">
+      <c r="O41" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maybe fixed trans file Segmentation Fault Bug, cause of MyList has some problem
</commit_message>
<xml_diff>
--- a/projects/MyTalk/MyTalk_protol.xlsx
+++ b/projects/MyTalk/MyTalk_protol.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25440" windowHeight="18735"/>
+    <workbookView windowWidth="27840" windowHeight="13350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57">
   <si>
     <t xml:space="preserve">
 </t>
@@ -104,9 +104,15 @@
     <t>S</t>
   </si>
   <si>
+    <t>tftp ip(string)</t>
+  </si>
+  <si>
     <t>返回注册信息</t>
   </si>
   <si>
+    <t>port(2byte)</t>
+  </si>
+  <si>
     <t>login ack:</t>
   </si>
   <si>
@@ -143,9 +149,6 @@
     <t>ip(string)</t>
   </si>
   <si>
-    <t>port(2byte)</t>
-  </si>
-  <si>
     <t>get friends ack:</t>
   </si>
   <si>
@@ -158,6 +161,9 @@
     <t>send msg:</t>
   </si>
   <si>
+    <t>发送消息</t>
+  </si>
+  <si>
     <t>0x0004</t>
   </si>
   <si>
@@ -168,6 +174,18 @@
   </si>
   <si>
     <t>msg(string)</t>
+  </si>
+  <si>
+    <t>client quit:</t>
+  </si>
+  <si>
+    <t>客户端退出处理，并发送退出消息给好友</t>
+  </si>
+  <si>
+    <t>head</t>
+  </si>
+  <si>
+    <t>0x0005</t>
   </si>
 </sst>
 </file>
@@ -175,12 +193,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -197,39 +215,49 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -248,103 +276,86 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -357,49 +368,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,133 +530,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,11 +562,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -579,32 +596,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -619,17 +610,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -648,157 +633,183 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -807,9 +818,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1126,10 +1134,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:XFD41"/>
+  <dimension ref="A1:XFD47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1236,7 +1244,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:13">
+    <row r="15" spans="2:15">
       <c r="B15" t="s">
         <v>24</v>
       </c>
@@ -1252,64 +1260,64 @@
       <c r="M15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="2:14">
+      <c r="O15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15">
       <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="N16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="15:17">
-      <c r="O17" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q17" t="s">
+      <c r="O16" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="14:14">
+      <c r="N17" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="15:17">
       <c r="O18" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="Q18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="14:14">
-      <c r="N21" t="s">
+    <row r="19" spans="15:17">
+      <c r="O19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="15:17">
-      <c r="O22" t="s">
+      <c r="Q19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="14:14">
+      <c r="N22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="15:17">
+      <c r="O23" t="s">
         <v>17</v>
       </c>
-      <c r="Q22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="15:15">
-      <c r="O23" t="s">
-        <v>36</v>
+      <c r="Q23" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="15:15">
       <c r="O24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="15:15">
       <c r="O25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="15:17">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="15:15">
       <c r="O26" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q26" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1318,65 +1326,96 @@
         <v>41</v>
       </c>
       <c r="Q27" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="15:17">
       <c r="O28" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q28" t="s">
         <v>42</v>
       </c>
-      <c r="Q28" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="14:14">
-      <c r="N31" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="15:17">
-      <c r="O32" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q32" t="s">
+    </row>
+    <row r="29" spans="15:17">
+      <c r="O29" t="s">
         <v>31</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="14:14">
+      <c r="N32" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="15:17">
       <c r="O33" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="Q33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="15:17">
+      <c r="O34" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="37" spans="14:14">
-      <c r="N37" t="s">
+      <c r="Q34" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="15:17">
-      <c r="O38" s="3" t="s">
+    <row r="38" spans="14:16">
+      <c r="N38" t="s">
+        <v>47</v>
+      </c>
+      <c r="P38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="15:17">
+      <c r="O39" t="s">
         <v>17</v>
       </c>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="15:15">
-      <c r="O39" t="s">
-        <v>48</v>
+      <c r="Q39" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="15:15">
       <c r="O40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="15:15">
       <c r="O41" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="15:15">
+      <c r="O42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="14:16">
+      <c r="N45" t="s">
+        <v>53</v>
+      </c>
+      <c r="P45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="15:17">
+      <c r="O46" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="15:15">
+      <c r="O47" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>